<commit_message>
fixed some latex bugs in DIG params
</commit_message>
<xml_diff>
--- a/utils/model2json/dig_information.xlsx
+++ b/utils/model2json/dig_information.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="322" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="322" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -721,7 +721,7 @@
     <t>VA_n</t>
   </si>
   <si>
-    <t>\text{valued added in NT sector}</t>
+    <t>\text{NT value add}</t>
   </si>
   <si>
     <t>value added in non-traded sector</t>
@@ -2103,8 +2103,8 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2781,8 +2781,8 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>